<commit_message>
Add country names for exogenous variables
</commit_message>
<xml_diff>
--- a/CountryConcordance.xlsx
+++ b/CountryConcordance.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanishka.Narayan\Desktop\FAOData\Aquastat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\PycharmProjects\WaterPreProcessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94A28887-82BB-4D87-9F32-1F449222DE23}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="257">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -707,19 +708,100 @@
     <t>Country Name in IFs</t>
   </si>
   <si>
-    <t>Area name</t>
-  </si>
-  <si>
     <t>Palestine</t>
   </si>
   <si>
     <t>Gambia, The</t>
+  </si>
+  <si>
+    <t>Bosnia</t>
+  </si>
+  <si>
+    <t>Central AfR</t>
+  </si>
+  <si>
+    <t>Congo; Republic of</t>
+  </si>
+  <si>
+    <t>Korea North</t>
+  </si>
+  <si>
+    <t>Congo; Democratic Republic of</t>
+  </si>
+  <si>
+    <t>DominicanRep</t>
+  </si>
+  <si>
+    <t>Equa Guinea</t>
+  </si>
+  <si>
+    <t>GuineaBiss</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Kyrgyz</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Micronesia; Fed. Sts.</t>
+  </si>
+  <si>
+    <t>Papua NG</t>
+  </si>
+  <si>
+    <t>Korea South</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>SierraLeo</t>
+  </si>
+  <si>
+    <t>Slovak Rep</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Trinidad</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>Unitd Kingdm</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Exogenous country name</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>AQUASTAT country name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -785,7 +867,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet2" xfId="1"/>
+    <cellStyle name="Normal_Sheet2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1062,1624 +1144,2259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B201"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
       <c r="B46" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
       <c r="B47" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
       <c r="B48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>60</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>61</v>
       </c>
       <c r="B53" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>62</v>
       </c>
       <c r="B54" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
       <c r="B56" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>66</v>
       </c>
       <c r="B57" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>67</v>
       </c>
       <c r="B58" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>68</v>
       </c>
       <c r="B59" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>69</v>
       </c>
       <c r="B60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>70</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
       <c r="B62" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>72</v>
       </c>
       <c r="B63" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
       <c r="B64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>74</v>
       </c>
       <c r="B65" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="C66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
       <c r="B67" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>77</v>
       </c>
       <c r="B68" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
       <c r="B69" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
       <c r="B70" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>80</v>
       </c>
       <c r="B71" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
       <c r="B72" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
       <c r="B73" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>83</v>
       </c>
       <c r="B74" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>84</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>85</v>
       </c>
       <c r="B76" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>87</v>
       </c>
       <c r="B78" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>88</v>
       </c>
       <c r="B79" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>89</v>
       </c>
       <c r="B80" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>90</v>
       </c>
       <c r="B81" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>91</v>
       </c>
       <c r="B82" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>94</v>
       </c>
       <c r="B84" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>95</v>
       </c>
       <c r="B85" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>97</v>
       </c>
       <c r="B87" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>98</v>
       </c>
       <c r="B88" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>99</v>
       </c>
       <c r="B89" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>100</v>
       </c>
       <c r="B90" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>101</v>
       </c>
       <c r="B91" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>102</v>
       </c>
       <c r="B92" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>103</v>
       </c>
       <c r="B93" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>104</v>
       </c>
       <c r="B94" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>105</v>
       </c>
       <c r="B95" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>107</v>
       </c>
       <c r="B96" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>109</v>
       </c>
       <c r="B97" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>110</v>
       </c>
       <c r="B98" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>111</v>
       </c>
       <c r="B99" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>112</v>
       </c>
       <c r="B100" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>113</v>
       </c>
       <c r="B101" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>114</v>
       </c>
       <c r="B102" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>115</v>
       </c>
       <c r="B103" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>116</v>
       </c>
       <c r="B104" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>117</v>
       </c>
       <c r="B105" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>118</v>
       </c>
       <c r="B106" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>119</v>
       </c>
       <c r="B107" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>120</v>
       </c>
       <c r="B108" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
       <c r="B109" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>122</v>
       </c>
       <c r="B110" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>123</v>
       </c>
       <c r="B111" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>124</v>
       </c>
       <c r="B112" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>125</v>
       </c>
       <c r="B113" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>126</v>
       </c>
       <c r="B114" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>127</v>
       </c>
       <c r="B115" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>128</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>129</v>
       </c>
       <c r="B117" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>130</v>
       </c>
       <c r="B118" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>131</v>
       </c>
       <c r="B119" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>132</v>
       </c>
       <c r="B120" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>133</v>
       </c>
       <c r="B121" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>134</v>
       </c>
       <c r="B122" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>135</v>
       </c>
       <c r="B123" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>136</v>
       </c>
       <c r="B124" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>137</v>
       </c>
       <c r="B125" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>138</v>
       </c>
       <c r="B126" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>139</v>
       </c>
       <c r="B127" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>140</v>
       </c>
       <c r="B128" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>141</v>
       </c>
       <c r="B129" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>142</v>
       </c>
       <c r="B130" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>143</v>
       </c>
       <c r="B131" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>144</v>
       </c>
       <c r="B132" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="C132" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>145</v>
       </c>
       <c r="B133" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>146</v>
       </c>
       <c r="B134" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>147</v>
       </c>
       <c r="B135" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>148</v>
       </c>
       <c r="B136" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>149</v>
       </c>
       <c r="B137" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>150</v>
       </c>
       <c r="B138" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>151</v>
       </c>
       <c r="B139" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>152</v>
       </c>
       <c r="B140" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>153</v>
       </c>
       <c r="B141" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>154</v>
       </c>
       <c r="B142" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>155</v>
       </c>
       <c r="B143" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>156</v>
       </c>
       <c r="B144" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>157</v>
       </c>
       <c r="B145" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>159</v>
       </c>
       <c r="B146" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>161</v>
       </c>
       <c r="B147" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>162</v>
       </c>
       <c r="B148" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>163</v>
       </c>
       <c r="B149" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>164</v>
       </c>
       <c r="B150" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>165</v>
       </c>
       <c r="B151" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>167</v>
       </c>
       <c r="B152" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>169</v>
       </c>
       <c r="B153" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>170</v>
       </c>
       <c r="B154" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>171</v>
       </c>
       <c r="B155" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>172</v>
       </c>
       <c r="B156" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>173</v>
       </c>
       <c r="B157" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>174</v>
       </c>
       <c r="B158" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>175</v>
       </c>
       <c r="B159" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>176</v>
       </c>
       <c r="B160" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>177</v>
       </c>
       <c r="B161" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>178</v>
       </c>
       <c r="B162" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>180</v>
       </c>
       <c r="B163" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>181</v>
       </c>
       <c r="B164" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>182</v>
       </c>
       <c r="B165" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>183</v>
       </c>
       <c r="B166" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>184</v>
       </c>
       <c r="B167" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>186</v>
       </c>
       <c r="B168" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>187</v>
       </c>
       <c r="B169" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>188</v>
       </c>
       <c r="B170" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>189</v>
       </c>
       <c r="B171" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>190</v>
       </c>
       <c r="B172" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>191</v>
       </c>
       <c r="B173" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>192</v>
       </c>
       <c r="B174" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>193</v>
       </c>
       <c r="B175" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>194</v>
       </c>
       <c r="B176" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>195</v>
       </c>
       <c r="B177" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>196</v>
       </c>
       <c r="B178" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>198</v>
       </c>
       <c r="B179" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>199</v>
       </c>
       <c r="B180" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>200</v>
       </c>
       <c r="B181" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>201</v>
       </c>
       <c r="B182" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>202</v>
       </c>
       <c r="B183" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>203</v>
       </c>
       <c r="B184" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>204</v>
       </c>
       <c r="B185" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>205</v>
       </c>
       <c r="B186" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>206</v>
       </c>
       <c r="B187" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C187" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>207</v>
       </c>
       <c r="B188" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>208</v>
       </c>
       <c r="B189" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C189" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>209</v>
       </c>
       <c r="B190" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>210</v>
       </c>
       <c r="B191" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>211</v>
       </c>
       <c r="B192" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C192" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>213</v>
       </c>
       <c r="B193" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C193" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>215</v>
       </c>
       <c r="B194" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C194" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>216</v>
       </c>
       <c r="B195" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C195" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>217</v>
       </c>
       <c r="B196" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C196" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>218</v>
       </c>
       <c r="B197" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C197" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>220</v>
       </c>
       <c r="B198" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C198" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>222</v>
       </c>
       <c r="B199" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>224</v>
       </c>
       <c r="B200" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C200" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>225</v>
       </c>
       <c r="B201" t="s">
         <v>225</v>
+      </c>
+      <c r="C201" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>253</v>
+      </c>
+      <c r="B202" t="s">
+        <v>253</v>
+      </c>
+      <c r="C202" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>254</v>
+      </c>
+      <c r="B203" t="s">
+        <v>254</v>
+      </c>
+      <c r="C203" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>255</v>
+      </c>
+      <c r="B204" t="s">
+        <v>255</v>
+      </c>
+      <c r="C204" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>